<commit_message>
feat: fix employee/leader names in Firestore to match Solides API
- Add updateEmployeeNameAndSolidesId and updateLeaderName to queries.ts
- Create migrate-names.ts script that updates existing Firestore data:
  - Corrects employee names to match Solides API exactly
  - Links solides_employee_id via slack_id cross-reference
  - Updates leader names and users collection
- Update seed.ts to link solides_employee_id during initial seeding
  using ID_solides_ID_slack.xlsx mapping
- Update seed-prod.ts to run migration on deploy when DB already seeded
- Fix mapeamento_final_com_slack.xlsx with correct Solides API names
  (69 employee names, 12 leader names corrected)

This ensures sync-punches.ts can match employees by name when
solides_employee_id is not yet linked, preventing missed punch records.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/mapeamento_final_com_slack.xlsx
+++ b/mapeamento_final_com_slack.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mapeamento_final" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="resumo_lideres" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="mapeamento_final" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="resumo_lideres" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -474,12 +474,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Rômulo Lisboa</t>
+          <t>Romulo Jose Santos Lisboa</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -492,21 +492,19 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>rômulo lisboa</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+          <t>romulo jose santos lisboa</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Rômulo Lisboa</t>
+          <t>Romulo Jose Santos Lisboa</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -519,11 +517,9 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>rômulo lisboa</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+          <t>romulo jose santos lisboa</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -533,7 +529,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ludmylla Wolpert</t>
+          <t>Ludmylla Wolpert Melo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -549,8 +545,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -560,7 +554,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rosilene Martins</t>
+          <t>Rosilene Martins Da Silva</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -576,8 +570,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -587,7 +579,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Anderson Rocha</t>
+          <t>Anderson Rosalvo Rocha dos Santos</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -603,8 +595,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -614,7 +604,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Márcio Alif Santos Silva</t>
+          <t>Marcio Alif Santos Silva</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -630,8 +620,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -641,7 +629,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Paulo Cesar</t>
+          <t>Paulo Cesar Da Silva Santos Junior</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -657,8 +645,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -668,7 +654,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Claudio</t>
+          <t>Claudio Bispo Dos Santos</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -684,8 +670,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -695,7 +679,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Danrley</t>
+          <t>Danrley firmino dos santos</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -711,8 +695,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -722,7 +704,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Luciano torres</t>
+          <t>Luciano Torres</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -738,8 +720,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -749,7 +729,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Thalys Gomes</t>
+          <t>Thalys Gomes Dos Santos</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -765,8 +745,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -776,7 +754,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>João victor</t>
+          <t>João Victor Santos da Silva</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -792,8 +770,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -819,8 +795,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -830,7 +804,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Pedro Lucas</t>
+          <t>Pedro Lucas Rocha da Fonseca</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -846,8 +820,6 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -857,7 +829,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Caique Santos</t>
+          <t>Caique dos santos da silva</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -873,18 +845,16 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Gessica Queiroz</t>
+          <t>Gessica Aparecida Dos Santos</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -897,21 +867,19 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Gessyca Nayara</t>
+          <t>Gessyca Nayara Rocha Santos</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -924,21 +892,19 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>lais manuelle</t>
+          <t>Laís Manuelle Santos Pereira</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -951,21 +917,19 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Kauanne Iwashita</t>
+          <t>Kauanne Iwashita Da Silva</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -978,21 +942,19 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Natali Gonzaga</t>
+          <t>Natali de Souza Gonzaga</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1005,21 +967,19 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nathália Vieira Lima</t>
+          <t>Nathalia Vieira Lima</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1032,21 +992,19 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Sabrina</t>
+          <t>Sabrina Domingos Santos</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1059,21 +1017,19 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Leticia Seixas</t>
+          <t>Leticia Seixas Santos</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1086,21 +1042,19 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Emanoelle Vieira</t>
+          <t>Emanoelle Feitosa Vieira Santos</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1113,21 +1067,19 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Giselle Santos Roberto</t>
+          <t>Giselle Dos Santos Roberto</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1140,21 +1092,19 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Joyce Cassimiro Souto</t>
+          <t>Joyce cassimiro souto</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1167,21 +1117,19 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ᗪᗩᐯᎥᗪ ᔕᎥᒪᐯᗩ</t>
+          <t>David da Silva Bento</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1194,21 +1142,19 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Kamilla Silva</t>
+          <t>Kamilla Santos da Silva</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1221,21 +1167,19 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>yuri castro</t>
+          <t>Yuri Castro Gomes</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1248,21 +1192,19 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Lucrécia Ferreira</t>
+          <t>Lucrécia Severo Ferreira</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1275,21 +1217,19 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Thalita Ruanna</t>
+          <t>Thalita Ruanna Santos Pereira</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1302,21 +1242,19 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Sandra Freitas</t>
+          <t>Sandra da Conceição Freitas</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1329,16 +1267,14 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1356,21 +1292,19 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>joão antonio</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
+          <t>joao antonio tavares santos</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Jordelle Meygre</t>
+          <t>Jordelle Meygre Costa De Oliveira</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1383,21 +1317,19 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>jonathan henrique</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
+          <t>jonathan henrique da conceição silva</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>EDNA</t>
+          <t>Edna Lopes Da Silva</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1410,21 +1342,19 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>jonathan henrique</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
+          <t>jonathan henrique da conceição silva</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Danielle</t>
+          <t>Danielle Dos Santos Silva</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1437,16 +1367,14 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>jonathan henrique</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
+          <t>jonathan henrique da conceição silva</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1464,21 +1392,19 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>jonathan henrique</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
+          <t>jonathan henrique da conceição silva</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Luan Backoffice Vd Palmeira</t>
+          <t>Luan Santos de Oliveira</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1491,21 +1417,19 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>jonathan henrique</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
+          <t>jonathan henrique da conceição silva</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Yasmim Barbosa</t>
+          <t>Yasmim Da Rocha Bezerra Barbosa</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1518,21 +1442,19 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>jonathan henrique</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
+          <t>jonathan henrique da conceição silva</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>João Ricardo</t>
+          <t>João Ricardo Dantas Albuquerque</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1545,21 +1467,19 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>jonathan henrique</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
+          <t>jonathan henrique da conceição silva</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Raquele Fragoso</t>
+          <t>Raquele Fragoso Da Silva</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1572,21 +1492,19 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>jonathan henrique</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
+          <t>jonathan henrique da conceição silva</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Maria Victória Araújo</t>
+          <t>Maria Victoria Souza Araujo Ferro</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1599,21 +1517,19 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>jonathan henrique</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
+          <t>jonathan henrique da conceição silva</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Camilla Emanuelle Lopes De Almeida</t>
+          <t>Camilla Emanuelle Lopes de Almeida</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1626,16 +1542,14 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>jonathan henrique</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
+          <t>jonathan henrique da conceição silva</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Carlos Oliveira</t>
+          <t>Carlos Eduardo Silva De Oliveira</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1653,11 +1567,9 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>carlos oliveira</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
+          <t>carlos eduardo silva de oliveira</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1683,8 +1595,6 @@
           <t>leidiane souza</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1694,7 +1604,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Erick Café</t>
+          <t>Erick Café Santos Júnior</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1710,8 +1620,6 @@
           <t>leidiane souza</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1721,7 +1629,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Kemilly Rafaelly</t>
+          <t>Kemilly Rafaelly Souza Silva</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1737,8 +1645,6 @@
           <t>leidiane souza</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1748,7 +1654,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Mariane Sousa</t>
+          <t>Mariane Santos Sousa</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1764,8 +1670,6 @@
           <t>leidiane souza</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1775,7 +1679,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Taciane Pereira</t>
+          <t>Maria Taciane Pereira Barbosa</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1791,18 +1695,16 @@
           <t>leidiane souza</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Erick Café</t>
+          <t>Erick Café Santos Júnior</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Camille Kauane</t>
+          <t>Camille Kauane Da Silva Nunes</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1815,21 +1717,19 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>erick café</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
+          <t>erick café santos júnior</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Erick Café</t>
+          <t>Erick Café Santos Júnior</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Eliene</t>
+          <t>Eliene Da Silva Santos</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1842,21 +1742,19 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>erick café</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
+          <t>erick café santos júnior</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Erick Café</t>
+          <t>Erick Café Santos Júnior</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Tatiane</t>
+          <t>Maria Tatiane Basto Cardoso</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1869,11 +1767,9 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>erick café</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
+          <t>erick café santos júnior</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1883,7 +1779,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Valesca Vitorio</t>
+          <t>Valesca Meirelle Bezerra Vitória</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1899,8 +1795,6 @@
           <t>leidiane souza.1</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1910,7 +1804,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Yasmin Abilia</t>
+          <t>Yasmin Abilia Ferro da Silva</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1926,8 +1820,6 @@
           <t>leidiane souza.1</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1937,7 +1829,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Robéria  Gilo</t>
+          <t>Robéria Gilo Da Silva</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1953,8 +1845,6 @@
           <t>leidiane souza.1</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1964,7 +1854,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Deise Gislaine</t>
+          <t>Deise Gislaine Silva vitor</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1980,8 +1870,6 @@
           <t>ana clara de matos chagas</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1991,7 +1879,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Cris</t>
+          <t>Cristielle Pereira Lima Da Silva</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2007,8 +1895,6 @@
           <t>ana clara de matos chagas</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2018,7 +1904,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>samyra anchieta</t>
+          <t>Samyra Anchieta Bispo</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2034,18 +1920,16 @@
           <t>ana clara de matos chagas</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Kemilly Rafaelly</t>
+          <t>Kemilly Rafaelly Souza Silva</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Gabrielle Vitoria</t>
+          <t>Gabrielle Vitoria dos Santos</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2058,21 +1942,19 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>kemilly rafaelly</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="inlineStr"/>
+          <t>kemilly rafaelly souza silva</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Kemilly Rafaelly</t>
+          <t>Kemilly Rafaelly Souza Silva</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Maryanna Trajano</t>
+          <t>Maryanna Francielly Trajano da Silva</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2085,21 +1967,19 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>kemilly rafaelly</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr"/>
+          <t>kemilly rafaelly souza silva</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Taciane Pereira</t>
+          <t>Maria Taciane Pereira Barbosa</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Thamirys Silvestrini</t>
+          <t>THAMIRYS SILVESTRINI MORALES</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2112,21 +1992,19 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>taciane pereira</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr"/>
+          <t>maria taciane pereira barbosa</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Taciane Pereira</t>
+          <t>Maria Taciane Pereira Barbosa</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Bruna Rayane</t>
+          <t>Bruna Rayane Oliveira dos Santos</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2139,21 +2017,19 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>taciane pereira</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="inlineStr"/>
+          <t>maria taciane pereira barbosa</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Taciane Pereira</t>
+          <t>Maria Taciane Pereira Barbosa</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Ana paula</t>
+          <t>Ana Paula Amaral Santos Ismerim</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2166,21 +2042,19 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>taciane pereira</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="inlineStr"/>
+          <t>maria taciane pereira barbosa</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Mariane Sousa</t>
+          <t>Mariane Santos Sousa</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Anny Karoline</t>
+          <t>Anny Karoline Andrade Santos</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2193,21 +2067,19 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>mariane sousa</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr"/>
-      <c r="G65" t="inlineStr"/>
+          <t>mariane santos sousa</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Michaell Jean Nunes de Carvalho</t>
+          <t>Michaell Jean Nunes De Carvalho</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Tomás Azevedo</t>
+          <t>Tomás Azevedo Santos</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2223,18 +2095,16 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Michaell Jean Nunes de Carvalho</t>
+          <t>Michaell Jean Nunes De Carvalho</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Maria Nobre</t>
+          <t>Maria Nobre Farias De França</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2250,18 +2120,16 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Michaell Jean Nunes de Carvalho</t>
+          <t>Michaell Jean Nunes De Carvalho</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Alyni</t>
+          <t>Alyni Mayara Farias Da Silva Santos</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2277,18 +2145,16 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Michaell Jean Nunes de Carvalho</t>
+          <t>Michaell Jean Nunes De Carvalho</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Mara</t>
+          <t>Josimara Ferreira Monteiro</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2304,18 +2170,16 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Michaell Jean Nunes de Carvalho</t>
+          <t>Michaell Jean Nunes De Carvalho</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>juliene</t>
+          <t>Juliene bezerra</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2331,18 +2195,16 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Michaell Jean Nunes de Carvalho</t>
+          <t>Michaell Jean Nunes De Carvalho</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Luis Henrique</t>
+          <t>Luís Henrique Batista dos Santos</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2358,13 +2220,11 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Rafaela Mendes</t>
+          <t>Rafaela Alves Mendes</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2382,21 +2242,19 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>rafaela mendes</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="inlineStr"/>
+          <t>rafaela alves mendes</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Rafaela Mendes</t>
+          <t>Rafaela Alves Mendes</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Millena Sthefany</t>
+          <t>Millena Sthefany dos Santos Cruz</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2409,21 +2267,19 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>rafaela mendes</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="inlineStr"/>
+          <t>rafaela alves mendes</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Suzana Tavares</t>
+          <t>Suzana Martins Tavares</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>ravy thiago</t>
+          <t>Ravy Thiago Vieira Da Silva</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2436,21 +2292,19 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>suzana tavares</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" t="inlineStr"/>
+          <t>suzana martins tavares</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Suzana Tavares</t>
+          <t>Suzana Martins Tavares</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Thayane Mayara</t>
+          <t>Thayane Mayara dos Santos</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2463,16 +2317,14 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>suzana tavares</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" t="inlineStr"/>
+          <t>suzana martins tavares</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Suzana Tavares</t>
+          <t>Suzana Martins Tavares</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2490,21 +2342,19 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>suzana tavares</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="inlineStr"/>
+          <t>suzana martins tavares</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>ravy thiago</t>
+          <t>Ravy Thiago Vieira Da Silva</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Thayane Mayara</t>
+          <t>Thayane Mayara dos Santos</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2517,20 +2367,19 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>ravy thiago</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr"/>
+          <t>ravy thiago vieira da silva</t>
+        </is>
+      </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Suzana Tavares</t>
+          <t>Suzana Martins Tavares</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>ravy thiago</t>
+          <t>Ravy Thiago Vieira Da Silva</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2548,13 +2397,12 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ravy thiago</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr"/>
+          <t>ravy thiago vieira da silva</t>
+        </is>
+      </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Suzana Tavares</t>
+          <t>Suzana Martins Tavares</t>
         </is>
       </c>
     </row>
@@ -2603,7 +2451,6 @@
       <c r="B2" t="n">
         <v>13</v>
       </c>
-      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2614,62 +2461,56 @@
       <c r="B3" t="n">
         <v>3</v>
       </c>
-      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Carlos Oliveira</t>
+          <t>Carlos Eduardo Silva De Oliveira</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Erick Café</t>
+          <t>Erick Café Santos Júnior</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Jonathan Henrique</t>
+          <t>Jonathan Henrique da Conceição Silva</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>10</v>
       </c>
-      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>João Antonio</t>
+          <t>Joao Antonio Tavares Santos</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>18</v>
       </c>
-      <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Kemilly Rafaelly</t>
+          <t>Kemilly Rafaelly Souza Silva</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>2</v>
       </c>
-      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2680,7 +2521,6 @@
       <c r="B9" t="n">
         <v>5</v>
       </c>
-      <c r="C9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2691,84 +2531,76 @@
       <c r="B10" t="n">
         <v>3</v>
       </c>
-      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mariane Sousa</t>
+          <t>Mariane Santos Sousa</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
-      <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Michaell Jean Nunes de Carvalho</t>
+          <t>Michaell Jean Nunes De Carvalho</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>6</v>
       </c>
-      <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Rafaela Mendes</t>
+          <t>Rafaela Alves Mendes</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>2</v>
       </c>
-      <c r="C13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Rômulo Lisboa</t>
+          <t>Romulo Jose Santos Lisboa</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>2</v>
       </c>
-      <c r="C14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Suzana Tavares</t>
+          <t>Suzana Martins Tavares</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>3</v>
       </c>
-      <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Taciane Pereira</t>
+          <t>Maria Taciane Pereira Barbosa</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>3</v>
       </c>
-      <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ravy thiago</t>
+          <t>Ravy Thiago Vieira Da Silva</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>2</v>
       </c>
-      <c r="C17" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix: update mapeamento Excel with leader Slack IDs
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/mapeamento_final_com_slack.xlsx
+++ b/mapeamento_final_com_slack.xlsx
@@ -495,6 +495,11 @@
           <t>romulo jose santos lisboa</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>U07LSKN7SNL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -520,6 +525,11 @@
           <t>romulo jose santos lisboa</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>U07LSKN7SNL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -545,6 +555,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -570,6 +585,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -595,6 +615,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -620,6 +645,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -645,6 +675,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -670,6 +705,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -695,6 +735,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -720,6 +765,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -745,6 +795,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -770,6 +825,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -795,6 +855,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -820,6 +885,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -845,6 +915,11 @@
           <t>alberto luiz marinho batista</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -870,6 +945,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -895,6 +975,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -920,6 +1005,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -945,6 +1035,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -970,6 +1065,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -995,6 +1095,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1020,6 +1125,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1045,6 +1155,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1070,6 +1185,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1095,6 +1215,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1120,6 +1245,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1145,6 +1275,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1170,6 +1305,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1195,6 +1335,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1220,6 +1365,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1245,6 +1395,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1270,6 +1425,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1295,6 +1455,11 @@
           <t>joao antonio tavares santos</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1320,6 +1485,11 @@
           <t>jonathan henrique da conceição silva</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>U07L4D3EWJW</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1345,6 +1515,11 @@
           <t>jonathan henrique da conceição silva</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>U07L4D3EWJW</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1370,6 +1545,11 @@
           <t>jonathan henrique da conceição silva</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>U07L4D3EWJW</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1395,6 +1575,11 @@
           <t>jonathan henrique da conceição silva</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>U07L4D3EWJW</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1420,6 +1605,11 @@
           <t>jonathan henrique da conceição silva</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>U07L4D3EWJW</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1445,6 +1635,11 @@
           <t>jonathan henrique da conceição silva</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>U07L4D3EWJW</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1470,6 +1665,11 @@
           <t>jonathan henrique da conceição silva</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>U07L4D3EWJW</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1495,6 +1695,11 @@
           <t>jonathan henrique da conceição silva</t>
         </is>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>U07L4D3EWJW</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1520,6 +1725,11 @@
           <t>jonathan henrique da conceição silva</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>U07L4D3EWJW</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1545,6 +1755,11 @@
           <t>jonathan henrique da conceição silva</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>U07L4D3EWJW</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1570,6 +1785,11 @@
           <t>carlos eduardo silva de oliveira</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>U0895CZ8HU7</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1595,6 +1815,11 @@
           <t>leidiane souza</t>
         </is>
       </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>U07KX76F7D4</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1620,6 +1845,11 @@
           <t>leidiane souza</t>
         </is>
       </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>U07KX76F7D4</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1645,6 +1875,11 @@
           <t>leidiane souza</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>U07KX76F7D4</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1670,6 +1905,11 @@
           <t>leidiane souza</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>U07KX76F7D4</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1695,6 +1935,11 @@
           <t>leidiane souza</t>
         </is>
       </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>U07KX76F7D4</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1720,6 +1965,11 @@
           <t>erick café santos júnior</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>U07KPE840MD</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1745,6 +1995,11 @@
           <t>erick café santos júnior</t>
         </is>
       </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>U07KPE840MD</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1770,6 +2025,11 @@
           <t>erick café santos júnior</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>U07KPE840MD</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1795,6 +2055,11 @@
           <t>leidiane souza.1</t>
         </is>
       </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>U07KX76F7D4</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1820,6 +2085,11 @@
           <t>leidiane souza.1</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>U07KX76F7D4</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1845,6 +2115,11 @@
           <t>leidiane souza.1</t>
         </is>
       </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>U07KX76F7D4</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1870,6 +2145,11 @@
           <t>ana clara de matos chagas</t>
         </is>
       </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>U08F9KK0AAG</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1895,6 +2175,11 @@
           <t>ana clara de matos chagas</t>
         </is>
       </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>U08F9KK0AAG</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1920,6 +2205,11 @@
           <t>ana clara de matos chagas</t>
         </is>
       </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>U08F9KK0AAG</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1945,6 +2235,11 @@
           <t>kemilly rafaelly souza silva</t>
         </is>
       </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>U087HDEARA9</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1970,6 +2265,11 @@
           <t>kemilly rafaelly souza silva</t>
         </is>
       </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>U087HDEARA9</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1995,6 +2295,11 @@
           <t>maria taciane pereira barbosa</t>
         </is>
       </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>U07L6EAUS75</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2020,6 +2325,11 @@
           <t>maria taciane pereira barbosa</t>
         </is>
       </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>U07L6EAUS75</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2045,6 +2355,11 @@
           <t>maria taciane pereira barbosa</t>
         </is>
       </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>U07L6EAUS75</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2070,6 +2385,11 @@
           <t>mariane santos sousa</t>
         </is>
       </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>U088B372R40</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2095,6 +2415,11 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>U07P692F1FB</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2120,6 +2445,11 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>U07P692F1FB</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2145,6 +2475,11 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>U07P692F1FB</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2170,6 +2505,11 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>U07P692F1FB</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2195,6 +2535,11 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>U07P692F1FB</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2220,6 +2565,11 @@
           <t>michaell jean nunes de carvalho</t>
         </is>
       </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>U07P692F1FB</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2245,6 +2595,11 @@
           <t>rafaela alves mendes</t>
         </is>
       </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>U07KP9J5BLP</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2270,6 +2625,11 @@
           <t>rafaela alves mendes</t>
         </is>
       </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>U07KP9J5BLP</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2295,6 +2655,11 @@
           <t>suzana martins tavares</t>
         </is>
       </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>U09F9LWM6MC</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2320,6 +2685,11 @@
           <t>suzana martins tavares</t>
         </is>
       </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>U09F9LWM6MC</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2345,6 +2715,11 @@
           <t>suzana martins tavares</t>
         </is>
       </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>U09F9LWM6MC</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2370,6 +2745,11 @@
           <t>ravy thiago vieira da silva</t>
         </is>
       </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>U07Q8NT7J1Y</t>
+        </is>
+      </c>
       <c r="G77" t="inlineStr">
         <is>
           <t>Suzana Martins Tavares</t>
@@ -2398,6 +2778,11 @@
       <c r="E78" t="inlineStr">
         <is>
           <t>ravy thiago vieira da silva</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>U07Q8NT7J1Y</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -2451,6 +2836,11 @@
       <c r="B2" t="n">
         <v>13</v>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>U07KXEJU338</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2461,6 +2851,11 @@
       <c r="B3" t="n">
         <v>3</v>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>U08F9KK0AAG</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2471,6 +2866,11 @@
       <c r="B4" t="n">
         <v>1</v>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>U0895CZ8HU7</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2481,6 +2881,11 @@
       <c r="B5" t="n">
         <v>3</v>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>U07KPE840MD</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2491,6 +2896,11 @@
       <c r="B6" t="n">
         <v>10</v>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>U07L4D3EWJW</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2501,6 +2911,11 @@
       <c r="B7" t="n">
         <v>18</v>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>U07LP4JSN9K</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2511,6 +2926,11 @@
       <c r="B8" t="n">
         <v>2</v>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>U087HDEARA9</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2521,6 +2941,11 @@
       <c r="B9" t="n">
         <v>5</v>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>U07KX76F7D4</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2541,6 +2966,11 @@
       <c r="B11" t="n">
         <v>1</v>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>U088B372R40</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2551,6 +2981,11 @@
       <c r="B12" t="n">
         <v>6</v>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>U07P692F1FB</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2561,6 +2996,11 @@
       <c r="B13" t="n">
         <v>2</v>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>U07KP9J5BLP</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2571,6 +3011,11 @@
       <c r="B14" t="n">
         <v>2</v>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>U07LSKN7SNL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2581,6 +3026,11 @@
       <c r="B15" t="n">
         <v>3</v>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>U09F9LWM6MC</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2591,6 +3041,11 @@
       <c r="B16" t="n">
         <v>3</v>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>U07L6EAUS75</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2600,6 +3055,11 @@
       </c>
       <c r="B17" t="n">
         <v>2</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>U07Q8NT7J1Y</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>